<commit_message>
add dedicated server binary
</commit_message>
<xml_diff>
--- a/docs/version_scheduling/0.1.0-pre1.xlsx
+++ b/docs/version_scheduling/0.1.0-pre1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mario\Zombono\docs\version_scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D00C64E-D5E4-4BB2-AF38-E11A2C229B5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB910747-160F-40E7-AB61-A980CEC9DAD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{D3954C5D-F7DA-4B2B-BA30-12E624254EF1}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="44">
   <si>
     <t>Task</t>
   </si>
@@ -535,7 +535,7 @@
   <dimension ref="A1:D32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+      <selection activeCell="D32" sqref="A1:D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -652,6 +652,12 @@
       <c r="B11" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="C11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="3">
+        <v>45472</v>
+      </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">

</xml_diff>